<commit_message>
modification pour mettre à jour IG par rapport à la maturité implémentation ROR 3.1  (#328)
* Update search_param.md

suppr draft et ajout SP identifer PR et PRRole cf issue + typo

* Update modifiers.md

suppr draft sur of-type cf issue

* add CapStt SP identifier Practitioner and PractitionerRole

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com>

* Update input/fsh/instances/ror-serveur.fsh

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com>

* correction description

* changement statut CS

---------

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com> 49390be3cc6e548f83388aa50ad4cbb711722629
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.1</t>
+    <t>0.3.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-29T09:39:56+00:00</t>
+    <t>2024-03-12T11:10:47+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
update version ci-build (#337)
* update version ci-build

* correction lien 03bb5593b9bf4ad9e49cb353c0caa9334511bebd
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.3.0</t>
+    <t>0.4.0-ballot-1</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-13T10:24:41+00:00</t>
+    <t>2024-03-13T16:27:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Sd add new ms questionnaire (#347)
* add new MS et short dans questionnaire 5709e55add6eff5fe596064d536e35269e135f8f
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-02T16:06:43+00:00</t>
+    <t>2024-04-10T16:04:08+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -66,7 +66,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>ANS (https://esante.gouv.fr)</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>

<commit_message>
preparation publication ballot (#354)
* preparation publication ballot

* Update release-notes.md b3d8ae07e3df2e38fe263b0f992d5edea5603e21
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -45,7 +45,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>active</t>
+    <t>draft</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-13T09:06:15+00:00</t>
+    <t>2024-05-15T15:09:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
add qa-preview label (#355) 548371cbf4236183efd85ec6548e9a8522fd1d3d
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.4.0-ballot-1</t>
+    <t>0.4.0-qa-preview-1</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-15T15:09:55+00:00</t>
+    <t>2024-05-16T12:22:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
preparation publication 0-4-0 (#391)
* prep publication

* narratif précision sur les POST c66af8823b56111eaee76270ef0f967c6577beb0
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.4.0-snapshot-2</t>
+    <t>0.4.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-05T09:03:52+00:00</t>
+    <t>2024-12-09T11:05:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Cp questionnaire usecontext (#393)
* Update RORQuestionnaire.fsh

* Update RORQuestionnaireOffreDeVille.fsh

* add shareablecodesystem in CS

* add shareablevalueset in VS

* add experimental 99b3414109904aeaa7c63045292a2efdbed4a51a
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Property</t>
   </si>
@@ -51,10 +51,13 @@
     <t>Experimental</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-22T15:00:55+00:00</t>
+    <t>2025-01-28T15:58:19+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -88,9 +91,6 @@
   </si>
   <si>
     <t>Case Sensitive</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>Value Set (all codes)</t>
@@ -341,66 +341,68 @@
       <c r="A7" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" t="s" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
Prep ig ror33 (#404)
* prep publication

version 0.5.0

* Update index.md b10467b2e0331c84ea6776b16422a7dc9b5d6695
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.5.0-snapshot-1</t>
+    <t>0.5.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-10T14:14:07+00:00</t>
+    <t>2025-03-13T17:00:51+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
update ci-build (#406) 2f9e84eb76abe98268cc1dcc97dbf2af56f163a6
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/main/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.5.0</t>
+    <t>0.6.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-17T13:12:35+00:00</t>
+    <t>2025-03-18T09:01:13+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>